<commit_message>
test: save files for testsuit
</commit_message>
<xml_diff>
--- a/test_docs/testsuite/info_page/wrong/no_source.xlsx
+++ b/test_docs/testsuite/info_page/wrong/no_source.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Nom source</t>
   </si>
@@ -50,10 +50,7 @@
     <t>n1</t>
   </si>
   <si>
-    <t>n2</t>
-  </si>
-  <si>
-    <t>o1</t>
+    <t/>
   </si>
 </sst>
 </file>
@@ -298,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -343,6 +340,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
@@ -712,12 +715,12 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1"/>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="16" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="D4" s="14" t="s">
-        <v>12</v>
+      <c r="D4" s="17" t="s">
+        <v>11</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="15"/>
@@ -796,11 +799,11 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="1"/>
-      <c r="B14" s="16"/>
+      <c r="B14" s="18"/>
       <c r="C14" s="7"/>
-      <c r="D14" s="17"/>
+      <c r="D14" s="19"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="18"/>
+      <c r="F14" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>